<commit_message>
Catch up to publication
</commit_message>
<xml_diff>
--- a/Data/USA/USA_bea_naics_map.xlsx
+++ b/Data/USA/USA_bea_naics_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dietz/Dropbox/Project/Elasticity/Data/USA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9A9F50-ACFB-AA45-A16F-B8DD94A52254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E32079-AC54-4242-A5A9-0BBB5ECCD948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{D31BAD4F-5CC4-7B4A-A5F0-1A155B16B683}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32080" windowHeight="19820" activeTab="1" xr2:uid="{D31BAD4F-5CC4-7B4A-A5F0-1A155B16B683}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -1187,19 +1187,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1527,106 +1525,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA84CB4-B346-E74B-B963-8A9BEEFA2392}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="6" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="6"/>
-    <col min="4" max="4" width="17.1640625" style="6" customWidth="1"/>
-    <col min="5" max="8" width="10.83203125" style="6"/>
-    <col min="9" max="9" width="40.83203125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="6"/>
+    <col min="1" max="1" width="10.6640625" style="5" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="5"/>
+    <col min="4" max="4" width="17.1640625" style="5" customWidth="1"/>
+    <col min="5" max="8" width="10.83203125" style="5"/>
+    <col min="9" max="9" width="40.83203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="12"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>190</v>
       </c>
     </row>
@@ -1639,1533 +1637,1532 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF1E61E4-9DF1-BA41-A8BE-9A8983E5FE77}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-    <col min="3" max="3" width="52.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="49.83203125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="52.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="49.83203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>2110</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>2120</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>2130</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>2200</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>2300</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>3210</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>3270</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>3310</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>3320</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>3330</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>3340</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>3350</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>3370</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>3220</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>3230</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>3240</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>3250</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>3260</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="4">
         <v>4200</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="1" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>4810</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="1" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>4820</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="1" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>4830</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="1" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>4840</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="1" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>4850</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="1" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>4860</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="1" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" s="1" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+      <c r="A40" s="3">
         <v>4930</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+      <c r="A41" s="3">
         <v>5110</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G41" s="1" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="A42" s="3">
         <v>5120</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E42" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="1" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+      <c r="A43" s="3">
         <v>5130</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E43" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="1" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+      <c r="A44" s="3">
         <v>5140</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E44" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G44" s="1" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
+      <c r="A45" s="2">
         <v>5210</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E45" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F45" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G45" s="1" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
+      <c r="A46" s="2">
         <v>5220</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G46" s="1" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+      <c r="A47" s="3">
         <v>5230</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G47" s="1" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+      <c r="A48" s="3">
         <v>5240</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E48" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F48" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G48" s="1" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
+      <c r="A49" s="3">
         <v>5250</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E49" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F49" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G49" s="1" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+      <c r="A50" s="3">
         <v>5310</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="E50" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="F50" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="G50" s="1" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+      <c r="A51" s="3">
         <v>5310</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
+      <c r="A52" s="3">
         <v>5320</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E52" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F52" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="G52" s="1" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
+      <c r="A53" s="3">
         <v>5411</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E53" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F53" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="G53" s="1" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
+      <c r="A54" s="3">
         <v>5415</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D54" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E54" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="F54" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="G54" s="1" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
+      <c r="A55" s="3">
         <v>5412</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E55" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="F55" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="G55" s="1" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
+      <c r="A56" s="3">
         <v>5500</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E56" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="F56" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="G56" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
+      <c r="A57" s="3">
         <v>5610</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D57" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="E57" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F57" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G57" s="2" t="s">
+      <c r="G57" s="1" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+      <c r="A58" s="3">
         <v>5620</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E58" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F58" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="G58" s="1" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
+      <c r="A59" s="3">
         <v>6100</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D59" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="E59" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="F59" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="G59" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
+      <c r="A60" s="3">
         <v>6210</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E60" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="F60" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="G60" s="1" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D61" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="F61" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="G61" s="1" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
+      <c r="A62" s="3">
         <v>6230</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D62" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="E62" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="F62" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="G62" s="1" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
+      <c r="A63" s="3">
         <v>6240</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D63" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="E63" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="F63" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="G63" s="1" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D64" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E64" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="F64" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G64" s="1" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="4">
+      <c r="A65" s="3">
         <v>7130</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D65" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="E65" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="F65" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G65" s="1" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="4">
+      <c r="A66" s="3">
         <v>7210</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D66" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="E66" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="F66" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="G66" s="1" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
+      <c r="A67" s="3">
         <v>7220</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D67" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="E67" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="F67" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="G67" s="1" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="4">
+      <c r="A68" s="3">
         <v>8100</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D68" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="E68" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="F68" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G68" s="2" t="s">
+      <c r="G68" s="1" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3173,10 +3170,10 @@
       <c r="A69" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C69" s="1" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3184,22 +3181,22 @@
       <c r="A70" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D70" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="E70" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="F70" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="G70" s="1" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3207,22 +3204,22 @@
       <c r="A71" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D71" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="E71" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="F71" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="G71" s="2" t="s">
+      <c r="G71" s="1" t="s">
         <v>149</v>
       </c>
     </row>
@@ -3230,22 +3227,22 @@
       <c r="A72" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D72" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="E72" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="F72" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G72" s="2" t="s">
+      <c r="G72" s="1" t="s">
         <v>151</v>
       </c>
     </row>
@@ -3253,22 +3250,22 @@
       <c r="A73" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C73" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D73" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="E73" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="F73" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G73" s="2" t="s">
+      <c r="G73" s="1" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3281,14 +3278,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F282F92C-5ED9-9343-8450-3C20F83A216B}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>192</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -3296,511 +3293,511 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>2110</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>2120</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>2130</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>2200</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>2300</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>3210</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>3270</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>3310</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>3320</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>3330</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>3340</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>3350</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>3370</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>3220</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>3230</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>3240</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>3250</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>3260</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="4">
         <v>4200</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="3">
         <v>4810</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <v>4820</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="3">
         <v>4830</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="3">
         <v>4840</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="3">
         <v>4850</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="3">
         <v>4860</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="3">
         <v>4930</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="3">
         <v>5110</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="3">
         <v>5120</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="3">
         <v>5130</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="3">
         <v>5140</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="2">
         <v>5210</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="2">
         <v>5220</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44" s="3">
         <v>5230</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45" s="3">
         <v>5240</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="3">
         <v>5250</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B47" s="4">
+      <c r="B47" s="3">
         <v>5310</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B48" s="3">
         <v>5320</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B49" s="3">
         <v>5411</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B50" s="3">
         <v>5415</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B51" s="3">
         <v>5412</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B52" s="4">
+      <c r="B52" s="3">
         <v>5500</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B53" s="4">
+      <c r="B53" s="3">
         <v>5610</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B54" s="4">
+      <c r="B54" s="3">
         <v>5620</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B55" s="4">
+      <c r="B55" s="3">
         <v>6100</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B56" s="4">
+      <c r="B56" s="3">
         <v>6210</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B58" s="4">
+      <c r="B58" s="3">
         <v>6230</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B59" s="4">
+      <c r="B59" s="3">
         <v>6240</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B61" s="3">
         <v>7130</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B62" s="4">
+      <c r="B62" s="3">
         <v>7210</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B63" s="4">
+      <c r="B63" s="3">
         <v>7220</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B64" s="3">
         <v>8100</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="1" t="s">
         <v>195</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -3808,7 +3805,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="1" t="s">
         <v>196</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -3824,7 +3821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37047228-AF18-3145-8F98-08BA73964554}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A73" sqref="A73:XFD74"/>
     </sheetView>
   </sheetViews>
@@ -3841,10 +3838,10 @@
       <c r="B1" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E1" t="s">
@@ -3861,10 +3858,10 @@
       <c r="B2" t="s">
         <v>200</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2">
@@ -3881,10 +3878,10 @@
       <c r="B3" t="s">
         <v>202</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E3" t="s">
@@ -3901,10 +3898,10 @@
       <c r="B4" t="s">
         <v>204</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E4" t="s">
@@ -3921,10 +3918,10 @@
       <c r="B5" t="s">
         <v>206</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E5" t="s">
@@ -3941,10 +3938,10 @@
       <c r="B6" t="s">
         <v>208</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
@@ -3961,10 +3958,10 @@
       <c r="B7" t="s">
         <v>210</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E7" t="s">
@@ -3981,10 +3978,10 @@
       <c r="B8" t="s">
         <v>212</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E8" t="s">
@@ -4001,10 +3998,10 @@
       <c r="B9" t="s">
         <v>214</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E9" t="s">
@@ -4021,10 +4018,10 @@
       <c r="B10" t="s">
         <v>216</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E10" t="s">
@@ -4041,10 +4038,10 @@
       <c r="B11" t="s">
         <v>218</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E11" t="s">
@@ -4061,10 +4058,10 @@
       <c r="B12" t="s">
         <v>220</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E12" t="s">
@@ -4081,10 +4078,10 @@
       <c r="B13" t="s">
         <v>222</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E13" t="s">
@@ -4101,10 +4098,10 @@
       <c r="B14" t="s">
         <v>224</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E14" t="s">
@@ -4121,10 +4118,10 @@
       <c r="B15" t="s">
         <v>226</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E15" t="s">
@@ -4141,10 +4138,10 @@
       <c r="B16" t="s">
         <v>227</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E16" t="s">
@@ -4161,10 +4158,10 @@
       <c r="B17" t="s">
         <v>228</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E17" t="s">
@@ -4181,10 +4178,10 @@
       <c r="B18" t="s">
         <v>230</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E18" t="s">
@@ -4201,10 +4198,10 @@
       <c r="B19" t="s">
         <v>232</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E19" t="s">
@@ -4221,10 +4218,10 @@
       <c r="B20" t="s">
         <v>234</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E20" t="s">
@@ -4241,10 +4238,10 @@
       <c r="B21" t="s">
         <v>236</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E21" t="s">
@@ -4261,10 +4258,10 @@
       <c r="B22" t="s">
         <v>238</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E22" t="s">
@@ -4281,10 +4278,10 @@
       <c r="B23" t="s">
         <v>240</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E23" t="s">
@@ -4301,10 +4298,10 @@
       <c r="B24" t="s">
         <v>242</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E24" t="s">
@@ -4321,10 +4318,10 @@
       <c r="B25" t="s">
         <v>244</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="1" t="s">
         <v>59</v>
       </c>
       <c r="E25" t="s">
@@ -4341,10 +4338,10 @@
       <c r="B26" t="s">
         <v>246</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E26" t="s">
@@ -4361,10 +4358,10 @@
       <c r="B27" t="s">
         <v>248</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E27" t="s">
@@ -4381,10 +4378,10 @@
       <c r="B28" t="s">
         <v>250</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E28" t="s">
@@ -4401,10 +4398,10 @@
       <c r="B29" t="s">
         <v>252</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="1" t="s">
         <v>67</v>
       </c>
       <c r="E29" t="s">
@@ -4421,10 +4418,10 @@
       <c r="B30" t="s">
         <v>254</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="1" t="s">
         <v>69</v>
       </c>
       <c r="E30" t="s">
@@ -4441,10 +4438,10 @@
       <c r="B31" t="s">
         <v>256</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E31" t="s">
@@ -4461,10 +4458,10 @@
       <c r="B32" t="s">
         <v>257</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="1" t="s">
         <v>73</v>
       </c>
       <c r="E32" t="s">
@@ -4481,10 +4478,10 @@
       <c r="B33" t="s">
         <v>259</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="1" t="s">
         <v>75</v>
       </c>
       <c r="E33" t="s">
@@ -4501,10 +4498,10 @@
       <c r="B34" t="s">
         <v>261</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E34" t="s">
@@ -4521,10 +4518,10 @@
       <c r="B35" t="s">
         <v>263</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="1" t="s">
         <v>79</v>
       </c>
       <c r="E35" t="s">
@@ -4541,10 +4538,10 @@
       <c r="B36" t="s">
         <v>265</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E36" t="s">
@@ -4561,10 +4558,10 @@
       <c r="B37" t="s">
         <v>266</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="1" t="s">
         <v>83</v>
       </c>
       <c r="E37" t="s">
@@ -4581,10 +4578,10 @@
       <c r="B38" t="s">
         <v>268</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="1" t="s">
         <v>85</v>
       </c>
       <c r="E38" t="s">
@@ -4601,10 +4598,10 @@
       <c r="B39" t="s">
         <v>270</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="1" t="s">
         <v>87</v>
       </c>
       <c r="E39" t="s">
@@ -4621,10 +4618,10 @@
       <c r="B40" t="s">
         <v>271</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="1" t="s">
         <v>89</v>
       </c>
       <c r="E40" t="s">
@@ -4641,10 +4638,10 @@
       <c r="B41" t="s">
         <v>273</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E41" t="s">
@@ -4661,10 +4658,10 @@
       <c r="B42" t="s">
         <v>274</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="1" t="s">
         <v>93</v>
       </c>
       <c r="E42" t="s">
@@ -4681,10 +4678,10 @@
       <c r="B43" t="s">
         <v>275</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E43" t="s">
@@ -4701,10 +4698,10 @@
       <c r="B44" t="s">
         <v>276</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E44" t="s">
@@ -4721,10 +4718,10 @@
       <c r="B45" t="s">
         <v>278</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="1" t="s">
         <v>99</v>
       </c>
       <c r="E45" t="s">
@@ -4741,10 +4738,10 @@
       <c r="B46" t="s">
         <v>280</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="1" t="s">
         <v>101</v>
       </c>
       <c r="E46" t="s">
@@ -4761,10 +4758,10 @@
       <c r="B47" t="s">
         <v>282</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="1" t="s">
         <v>103</v>
       </c>
       <c r="E47" t="s">
@@ -4781,10 +4778,10 @@
       <c r="B48" t="s">
         <v>283</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="1" t="s">
         <v>105</v>
       </c>
       <c r="E48" t="s">
@@ -4801,10 +4798,10 @@
       <c r="B49" t="s">
         <v>285</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="1" t="s">
         <v>109</v>
       </c>
       <c r="E49" t="s">
@@ -4821,10 +4818,10 @@
       <c r="B50" t="s">
         <v>352</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="1" t="s">
         <v>107</v>
       </c>
       <c r="E50">
@@ -4841,10 +4838,10 @@
       <c r="B51" t="s">
         <v>287</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="1" t="s">
         <v>111</v>
       </c>
       <c r="E51" t="s">
@@ -4861,10 +4858,10 @@
       <c r="B52" t="s">
         <v>289</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" s="1" t="s">
         <v>113</v>
       </c>
       <c r="E52" t="s">
@@ -4881,10 +4878,10 @@
       <c r="B53" t="s">
         <v>291</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="1" t="s">
         <v>115</v>
       </c>
       <c r="E53" t="s">
@@ -4901,10 +4898,10 @@
       <c r="B54" t="s">
         <v>293</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D54" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E54" t="s">
@@ -4921,10 +4918,10 @@
       <c r="B55" t="s">
         <v>295</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="1" t="s">
         <v>119</v>
       </c>
       <c r="E55" t="s">
@@ -4941,10 +4938,10 @@
       <c r="B56" t="s">
         <v>296</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="1" t="s">
         <v>121</v>
       </c>
       <c r="E56" t="s">
@@ -4961,10 +4958,10 @@
       <c r="B57" t="s">
         <v>298</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D57" s="1" t="s">
         <v>123</v>
       </c>
       <c r="E57" t="s">
@@ -4981,10 +4978,10 @@
       <c r="B58" t="s">
         <v>300</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" s="1" t="s">
         <v>125</v>
       </c>
       <c r="E58" t="s">
@@ -5001,10 +4998,10 @@
       <c r="B59" t="s">
         <v>302</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D59" s="1" t="s">
         <v>127</v>
       </c>
       <c r="E59" t="s">
@@ -5021,10 +5018,10 @@
       <c r="B60" t="s">
         <v>304</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" s="1" t="s">
         <v>129</v>
       </c>
       <c r="E60" t="s">
@@ -5041,10 +5038,10 @@
       <c r="B61" t="s">
         <v>306</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D61" s="1" t="s">
         <v>131</v>
       </c>
       <c r="E61" t="s">
@@ -5061,10 +5058,10 @@
       <c r="B62" t="s">
         <v>308</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D62" s="1" t="s">
         <v>133</v>
       </c>
       <c r="E62" t="s">
@@ -5081,10 +5078,10 @@
       <c r="B63" t="s">
         <v>310</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D63" s="1" t="s">
         <v>135</v>
       </c>
       <c r="E63" t="s">
@@ -5101,10 +5098,10 @@
       <c r="B64" t="s">
         <v>311</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D64" s="1" t="s">
         <v>137</v>
       </c>
       <c r="E64" t="s">
@@ -5121,10 +5118,10 @@
       <c r="B65" t="s">
         <v>313</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D65" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E65" t="s">
@@ -5141,10 +5138,10 @@
       <c r="B66" t="s">
         <v>315</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D66" s="1" t="s">
         <v>141</v>
       </c>
       <c r="E66" t="s">
@@ -5161,10 +5158,10 @@
       <c r="B67" t="s">
         <v>317</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D67" s="1" t="s">
         <v>143</v>
       </c>
       <c r="E67" t="s">
@@ -5181,10 +5178,10 @@
       <c r="B68" t="s">
         <v>320</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D68" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E68">
@@ -5201,10 +5198,10 @@
       <c r="B69" t="s">
         <v>322</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C69" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D69" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E69">
@@ -5221,10 +5218,10 @@
       <c r="B70" t="s">
         <v>324</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D70" s="1" t="s">
         <v>149</v>
       </c>
       <c r="E70">
@@ -5241,10 +5238,10 @@
       <c r="B71" t="s">
         <v>318</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D71" s="1" t="s">
         <v>151</v>
       </c>
       <c r="E71">
@@ -5261,10 +5258,10 @@
       <c r="B72" t="s">
         <v>327</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D72" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E72">
@@ -5283,7 +5280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D332D8B-E13B-6940-B068-884696EF34DF}">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>

</xml_diff>